<commit_message>
modified:   my stuff/cmse/finances/finances review.ipynb 	modified:   my stuff/cmse/finances/finances1.xlsx
</commit_message>
<xml_diff>
--- a/my stuff/cmse/finances/finances1.xlsx
+++ b/my stuff/cmse/finances/finances1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\finances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\the actual coding folder\cautious-adventure\my stuff\cmse\finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD19125-B2CF-45DC-93B8-45BE6633890C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A51CC7-445C-4CDD-9D9B-521E700B9759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXPORT" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="190">
   <si>
     <t>Date</t>
   </si>
@@ -1675,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="92" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A140" zoomScale="92" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1861,6 +1861,9 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
       <c r="D14">
         <v>-43</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>118</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="D33">
         <v>-37.090000000000003</v>
@@ -4316,8 +4319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5863529-F62E-438E-94F8-2070869BB322}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>